<commit_message>
add PA to codes
</commit_message>
<xml_diff>
--- a/inst/extdata/codes.xlsx
+++ b/inst/extdata/codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronrendahl/Sandbox/BaseballScorecard/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CD27D0-BB8B-D748-A688-82E52A348DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720FC401-4D9E-8849-9CAE-1E066A9FB16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="500" windowWidth="21760" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="17460" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="codes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="112">
   <si>
     <t>Pitch</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>NoPitch</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
@@ -727,7 +730,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -743,12 +746,13 @@
     <col min="3" max="3" width="8.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -765,16 +769,19 @@
         <v>102</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -787,11 +794,11 @@
       <c r="D2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -801,11 +808,14 @@
       <c r="C3" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -818,14 +828,17 @@
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -838,14 +851,17 @@
       <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -858,14 +874,17 @@
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="F6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -881,11 +900,14 @@
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -898,14 +920,17 @@
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -918,14 +943,17 @@
       <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -938,14 +966,17 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -958,14 +989,17 @@
       <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="F11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -978,11 +1012,14 @@
       <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -995,14 +1032,17 @@
       <c r="E13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1015,14 +1055,17 @@
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1035,14 +1078,17 @@
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="F15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1058,14 +1104,17 @@
       <c r="E16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="F16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1081,14 +1130,17 @@
       <c r="E17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="F17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -1104,11 +1156,14 @@
       <c r="E18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -1124,14 +1179,17 @@
       <c r="E19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" s="2">
         <v>1</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1147,14 +1205,17 @@
       <c r="E20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="2">
         <v>2</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -1170,14 +1231,17 @@
       <c r="E21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="2">
-        <v>3</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1193,14 +1257,17 @@
       <c r="E22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" s="2">
         <v>4</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>107</v>
       </c>
@@ -1216,14 +1283,17 @@
       <c r="E23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="2">
         <v>4</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -1236,11 +1306,14 @@
       <c r="D24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1253,11 +1326,14 @@
       <c r="D25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -1270,11 +1346,14 @@
       <c r="D26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="F26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -1287,11 +1366,14 @@
       <c r="D27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -1307,11 +1389,14 @@
       <c r="E28" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="F28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -1324,11 +1409,14 @@
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -1341,11 +1429,14 @@
       <c r="D30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -1358,11 +1449,14 @@
       <c r="D31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -1378,11 +1472,14 @@
       <c r="E32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -1398,11 +1495,14 @@
       <c r="E33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -1416,7 +1516,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -1430,7 +1530,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -1444,7 +1544,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -1458,7 +1558,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -1472,7 +1572,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -1486,7 +1586,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -1500,7 +1600,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1514,7 +1614,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1528,7 +1628,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -1545,7 +1645,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -1559,7 +1659,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -1573,7 +1673,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -1590,7 +1690,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1604,7 +1704,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
have advance use the same codes
</commit_message>
<xml_diff>
--- a/inst/extdata/codes.xlsx
+++ b/inst/extdata/codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronrendahl/Sandbox/BaseballScorecard/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CE2736-13BC-EA4B-B2BD-010BF7F27C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC021471-52AC-394A-B31B-BF739349482C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31460" yWindow="-1760" windowWidth="21720" windowHeight="18280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="codes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="111">
   <si>
     <t>Pitch</t>
   </si>
@@ -320,21 +320,12 @@
     <t>Safe on Steal, by Fielder's Choice</t>
   </si>
   <si>
-    <t>AOE</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>AX</t>
-  </si>
-  <si>
     <t>TB</t>
   </si>
   <si>
@@ -372,6 +363,9 @@
   </si>
   <si>
     <t>ROE</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -736,10 +730,10 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
+      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -761,25 +755,25 @@
         <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
@@ -790,7 +784,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
@@ -799,7 +793,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -810,13 +804,13 @@
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -833,10 +827,10 @@
         <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>3</v>
@@ -856,10 +850,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>3</v>
@@ -879,10 +873,10 @@
         <v>17</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>3</v>
@@ -890,7 +884,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
@@ -905,7 +899,7 @@
         <v>19</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>50</v>
@@ -928,10 +922,10 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>3</v>
@@ -951,10 +945,10 @@
         <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>3</v>
@@ -974,10 +968,10 @@
         <v>15</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>3</v>
@@ -997,10 +991,10 @@
         <v>14</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>3</v>
@@ -1020,7 +1014,7 @@
         <v>19</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>50</v>
@@ -1043,7 +1037,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>48</v>
@@ -1066,7 +1060,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>48</v>
@@ -1089,7 +1083,7 @@
         <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>48</v>
@@ -1115,10 +1109,10 @@
         <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>3</v>
@@ -1141,7 +1135,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>48</v>
@@ -1167,7 +1161,7 @@
         <v>19</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>50</v>
@@ -1193,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H19" s="2">
         <v>1</v>
@@ -1219,7 +1213,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H20" s="2">
         <v>2</v>
@@ -1245,7 +1239,7 @@
         <v>6</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H21" s="2">
         <v>3</v>
@@ -1271,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H22" s="2">
         <v>4</v>
@@ -1282,7 +1276,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
@@ -1297,7 +1291,7 @@
         <v>7</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H23" s="2">
         <v>4</v>
@@ -1320,7 +1314,7 @@
         <v>16</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>3</v>
@@ -1340,10 +1334,10 @@
         <v>11</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>3</v>
@@ -1363,7 +1357,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>9</v>
@@ -1383,7 +1377,7 @@
         <v>8</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>9</v>
@@ -1406,10 +1400,10 @@
         <v>42</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1426,10 +1420,10 @@
         <v>38</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>3</v>
@@ -1449,10 +1443,10 @@
         <v>39</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>3</v>
@@ -1472,10 +1466,10 @@
         <v>20</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>3</v>
@@ -1495,13 +1489,13 @@
         <v>20</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>3</v>
@@ -1521,13 +1515,13 @@
         <v>20</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>3</v>
@@ -1544,7 +1538,7 @@
         <v>27</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -1586,7 +1580,7 @@
         <v>11</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -1600,7 +1594,7 @@
         <v>29</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -1614,7 +1608,7 @@
         <v>30</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -1628,7 +1622,7 @@
         <v>31</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -1642,7 +1636,7 @@
         <v>16</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -1656,7 +1650,7 @@
         <v>14</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -1670,7 +1664,7 @@
         <v>32</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>32</v>
@@ -1715,7 +1709,7 @@
         <v>44</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>44</v>
@@ -1732,7 +1726,7 @@
         <v>90</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -1746,7 +1740,7 @@
         <v>45</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1760,7 +1754,7 @@
         <v>37</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use K+ for combined dropped third strike
</commit_message>
<xml_diff>
--- a/inst/extdata/codes.xlsx
+++ b/inst/extdata/codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronrendahl/Sandbox/BaseballScorecard/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC021471-52AC-394A-B31B-BF739349482C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F119CE74-03BD-7A4D-92BE-9A55F4B9B4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="112">
   <si>
     <t>Pitch</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>K+</t>
   </si>
 </sst>
 </file>
@@ -730,10 +733,10 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1468,6 +1471,9 @@
       <c r="E31" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="F31" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="G31" s="2" t="s">
         <v>107</v>
       </c>
@@ -1486,13 +1492,13 @@
         <v>32</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>107</v>
@@ -1512,13 +1518,13 @@
         <v>44</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>107</v>
@@ -1664,9 +1670,6 @@
         <v>32</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1709,9 +1712,6 @@
         <v>44</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="2" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
make FC codes separate
</commit_message>
<xml_diff>
--- a/inst/extdata/codes.xlsx
+++ b/inst/extdata/codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronrendahl/Sandbox/BaseballScorecard/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A804A9EE-3B37-E745-9391-3254DCADE18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E378E8E-1E02-4148-8680-07B0F17DFBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1180" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="codes" sheetId="1" r:id="rId1"/>
@@ -745,10 +745,10 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1813,7 +1813,7 @@
         <v>45</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1827,7 +1827,7 @@
         <v>37</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change advances to have A
</commit_message>
<xml_diff>
--- a/inst/extdata/codes.xlsx
+++ b/inst/extdata/codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronrendahl/Sandbox/BaseballScorecard/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E378E8E-1E02-4148-8680-07B0F17DFBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB88B27-BC23-9B4D-9EF9-EF9A75955B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="2420" windowWidth="25840" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="codes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="120">
   <si>
     <t>Pitch</t>
   </si>
@@ -365,9 +365,6 @@
     <t>ROE</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>K+</t>
   </si>
   <si>
@@ -381,6 +378,21 @@
   </si>
   <si>
     <t>Advance_</t>
+  </si>
+  <si>
+    <t>AFC</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>APB</t>
+  </si>
+  <si>
+    <t>AWP</t>
+  </si>
+  <si>
+    <t>AX</t>
   </si>
 </sst>
 </file>
@@ -745,10 +757,10 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -798,7 +810,7 @@
         <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -950,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -976,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1002,7 +1014,7 @@
         <v>3</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1028,7 +1040,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1054,7 +1066,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1127,7 +1139,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1156,7 +1168,7 @@
         <v>3</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1185,7 +1197,7 @@
         <v>3</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1214,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1417,7 +1429,7 @@
         <v>9</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1440,7 +1452,7 @@
         <v>9</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1466,7 +1478,7 @@
         <v>106</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1492,7 +1504,7 @@
         <v>3</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1536,7 +1548,7 @@
         <v>109</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>107</v>
@@ -1545,7 +1557,7 @@
         <v>3</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1565,7 +1577,7 @@
         <v>109</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>107</v>
@@ -1574,7 +1586,7 @@
         <v>3</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1594,7 +1606,7 @@
         <v>109</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>107</v>
@@ -1603,7 +1615,7 @@
         <v>3</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1617,7 +1629,7 @@
         <v>27</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1659,7 +1671,7 @@
         <v>11</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1673,7 +1685,7 @@
         <v>29</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1687,7 +1699,7 @@
         <v>30</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1701,7 +1713,7 @@
         <v>31</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1715,7 +1727,7 @@
         <v>16</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -1729,7 +1741,7 @@
         <v>14</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -1743,7 +1755,7 @@
         <v>32</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -1785,7 +1797,7 @@
         <v>44</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -1799,7 +1811,7 @@
         <v>90</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add Manfred men on 2 and 3
</commit_message>
<xml_diff>
--- a/inst/extdata/codes.xlsx
+++ b/inst/extdata/codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronrendahl/Sandbox/BaseballScorecard/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB88B27-BC23-9B4D-9EF9-EF9A75955B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91B6B8A-946A-0E49-91EF-C9598AF28919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="2420" windowWidth="25840" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="124">
   <si>
     <t>Pitch</t>
   </si>
@@ -393,6 +393,18 @@
   </si>
   <si>
     <t>AX</t>
+  </si>
+  <si>
+    <t>Manfred Man to 2B</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>Manfred Man to 3B</t>
+  </si>
+  <si>
+    <t>M3</t>
   </si>
 </sst>
 </file>
@@ -754,13 +766,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -829,76 +841,74 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>107</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3"/>
       <c r="J3" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>105</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4"/>
       <c r="J4" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>17</v>
@@ -915,25 +925,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G7" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>3</v>
@@ -941,68 +948,65 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>49</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>107</v>
@@ -1019,16 +1023,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>107</v>
@@ -1045,22 +1049,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>3</v>
@@ -1071,63 +1075,68 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>107</v>
@@ -1138,54 +1147,43 @@
       <c r="J15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>107</v>
@@ -1202,25 +1200,25 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>3</v>
@@ -1231,79 +1229,83 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H19" s="2">
-        <v>1</v>
+      <c r="I19" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K19" s="2"/>
+      <c r="K19" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="2">
-        <v>2</v>
+      <c r="I20" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="2"/>
+      <c r="K20" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>107</v>
       </c>
       <c r="H21" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>3</v>
@@ -1312,25 +1314,25 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>107</v>
       </c>
       <c r="H22" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>3</v>
@@ -1339,25 +1341,25 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>107</v>
       </c>
       <c r="H23" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>3</v>
@@ -1366,19 +1368,25 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>107</v>
+      </c>
+      <c r="H24" s="2">
+        <v>4</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>3</v>
@@ -1387,22 +1395,25 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>107</v>
+      </c>
+      <c r="H25" s="2">
+        <v>4</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>3</v>
@@ -1411,71 +1422,67 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>107</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>107</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>107</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>112</v>
@@ -1483,25 +1490,22 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>107</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>112</v>
@@ -1509,47 +1513,46 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>109</v>
+        <v>8</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>107</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K30" s="2"/>
+        <v>106</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="G31" s="2" t="s">
         <v>107</v>
       </c>
@@ -1562,45 +1565,40 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="G32" s="2" t="s">
         <v>107</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>109</v>
@@ -1620,83 +1618,113 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>119</v>
+        <v>32</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>81</v>
+        <v>110</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>116</v>
+        <v>19</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>116</v>
+        <v>28</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>116</v>
@@ -1704,13 +1732,13 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>116</v>
@@ -1718,127 +1746,155 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>118</v>
+        <v>33</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>116</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>